<commit_message>
files that didnt get merged in but should be updated to 3.4.3
</commit_message>
<xml_diff>
--- a/InputData/bldgs/EoCEDwEC/Elast of Component E Demand wrt E Cost.xlsx
+++ b/InputData/bldgs/EoCEDwEC/Elast of Component E Demand wrt E Cost.xlsx
@@ -1,34 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/nathaniyer/library/containers/com.microsoft.excel/data/state-eps-data-repository/template_state/bldgs/eocedwec/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\bldgs\EoCEDwEC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541AAFA7-2790-E648-B0BB-05B847927EA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="460" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="19425" windowHeight="11025" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="EIA Table 1" sheetId="2" r:id="rId2"/>
     <sheet name="EoCEDwEC" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -197,7 +185,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -379,7 +367,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -419,7 +407,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -514,23 +501,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -566,23 +536,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -758,27 +711,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="67.5" customWidth="1"/>
+    <col min="2" max="2" width="67.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27">
-        <v>44307</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -786,134 +736,134 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>2014</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -921,35 +871,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.5" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>5</v>
       </c>
@@ -960,7 +910,7 @@
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="4" t="s">
         <v>13</v>
@@ -973,7 +923,7 @@
       <c r="F5" s="5"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>6</v>
       </c>
@@ -996,7 +946,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>10</v>
       </c>
@@ -1019,7 +969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>11</v>
       </c>
@@ -1042,7 +992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>12</v>
       </c>
@@ -1065,7 +1015,7 @@
         <v>-0.22</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>15</v>
       </c>
@@ -1076,7 +1026,7 @@
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="4" t="s">
         <v>13</v>
@@ -1089,7 +1039,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>6</v>
       </c>
@@ -1112,7 +1062,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>10</v>
       </c>
@@ -1135,7 +1085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>11</v>
       </c>
@@ -1158,7 +1108,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>12</v>
       </c>
@@ -1187,7 +1137,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -1197,14 +1147,14 @@
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" customWidth="1"/>
-    <col min="2" max="3" width="17.1640625" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="2" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>46</v>
       </c>
@@ -1218,7 +1168,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1235,7 +1185,7 @@
         <v>-0.11000000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1252,7 +1202,7 @@
         <v>-0.13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1269,7 +1219,7 @@
         <v>-0.27999999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1286,7 +1236,7 @@
         <v>-0.13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1301,7 +1251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1315,7 +1265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1332,7 +1282,7 @@
         <v>-0.13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1349,7 +1299,7 @@
         <v>-0.13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -1366,7 +1316,7 @@
         <v>-0.27999999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>

</xml_diff>